<commit_message>
criando as tabelas para as abas adicionais do relatorio
</commit_message>
<xml_diff>
--- a/REFERENCIAS/Relatorio Anual.xlsx
+++ b/REFERENCIAS/Relatorio Anual.xlsx
@@ -4,17 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21108" windowHeight="13464"/>
+    <workbookView windowWidth="12108" windowHeight="8004" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Posição - Ações" sheetId="1" r:id="rId1"/>
+    <sheet name="Posição - BDR" sheetId="2" r:id="rId2"/>
+    <sheet name="Produto Tipo de Evento Valor lí" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="122">
   <si>
     <t>Produto</t>
   </si>
@@ -305,6 +307,81 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MELI34 - MERCADOLIBRE INC                                  </t>
+  </si>
+  <si>
+    <t>MELI34</t>
+  </si>
+  <si>
+    <t>BRMELIBDR006 - 101</t>
+  </si>
+  <si>
+    <t>BDR</t>
+  </si>
+  <si>
+    <t>BANCO B3 S.A.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NUBR33 - NU HOLDINGS LTD.                                  </t>
+  </si>
+  <si>
+    <t>NUBR33</t>
+  </si>
+  <si>
+    <t>BRNUBRBDR002 - 100</t>
+  </si>
+  <si>
+    <t>Tipo de Evento</t>
+  </si>
+  <si>
+    <t>Valor líquido</t>
+  </si>
+  <si>
+    <t>AGRO3 - BRASILAGRO CIA BRASILEIRA DE PROP AGRICOLAS</t>
+  </si>
+  <si>
+    <t>Dividendo</t>
+  </si>
+  <si>
+    <t>B3SA3 - B3 S.A. – BRASIL, BOLSA, BALCÃO</t>
+  </si>
+  <si>
+    <t>BRML3 - BR MALLS PARTICIPACOES S/A</t>
+  </si>
+  <si>
+    <t>CPLE6 - COMPANHIA PARANAENSE DE ENERGIA-COPEL</t>
+  </si>
+  <si>
+    <t>EZTC3 - EZ TEC EMPREENDIMENTO E PARTICIPACOES S.A.</t>
+  </si>
+  <si>
+    <t>FLRY3 - FLEURY S.A.</t>
+  </si>
+  <si>
+    <t>GGBR4 - GERDAU S.A.</t>
+  </si>
+  <si>
+    <t>INTB3 - INTELBRAS SA IND DE TELECOMUNICACAO ELETRONIC</t>
+  </si>
+  <si>
+    <t>PETR4 - PETROLEO BRASILEIRO S/A PETROBRAS</t>
+  </si>
+  <si>
+    <t>SAPR11 - CIA DE SANEAMENTO DO PARANA - SANEPAR</t>
+  </si>
+  <si>
+    <t>TAEE11 - TRANSMISSORA ALIANCA DE ENERGIA ELETRICA S/A</t>
+  </si>
+  <si>
+    <t>VALE3 - VALE S.A.</t>
+  </si>
+  <si>
+    <t>Juros Sobre Capital Próprio</t>
+  </si>
+  <si>
+    <t>CSMG3 - COMPANHIA DE SANEAMENTO DE MINAS GERAIS COPASA MG</t>
   </si>
 </sst>
 </file>
@@ -327,17 +404,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Segoe UI"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Segoe UI"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -961,23 +1038,32 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1515,7 +1601,7 @@
   <sheetPr/>
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -1535,945 +1621,1501 @@
   </cols>
   <sheetData>
     <row r="1" ht="33.6" spans="1:14">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" ht="43.2" spans="1:14">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="7">
         <v>6</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="7">
         <v>6</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="5">
+      <c r="K2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="10">
         <v>29.96</v>
       </c>
-      <c r="N2" s="5">
+      <c r="N2" s="10">
         <v>179.76</v>
       </c>
     </row>
     <row r="3" ht="43.2" spans="1:14">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="7">
         <v>35</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="7">
         <v>35</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" s="5">
+      <c r="K3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="10">
         <v>13.21</v>
       </c>
-      <c r="N3" s="5">
+      <c r="N3" s="10">
         <v>462.35</v>
       </c>
     </row>
     <row r="4" ht="43.2" spans="1:14">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="7">
         <v>20</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="7">
         <v>20</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M4" s="5">
+      <c r="K4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" s="10">
         <v>8.3</v>
       </c>
-      <c r="N4" s="5">
+      <c r="N4" s="10">
         <v>166</v>
       </c>
     </row>
     <row r="5" ht="43.2" spans="1:14">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="7">
         <v>20</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="7">
         <v>20</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M5" s="5">
+      <c r="K5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" s="10">
         <v>7.91</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="10">
         <v>158.2</v>
       </c>
     </row>
     <row r="6" ht="43.2" spans="1:14">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="7">
         <v>8</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="7">
         <v>8</v>
       </c>
-      <c r="K6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M6" s="5">
+      <c r="K6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" s="10">
         <v>15.69</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="10">
         <v>125.52</v>
       </c>
     </row>
     <row r="7" ht="43.2" spans="1:14">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="7">
         <v>10</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="7">
         <v>10</v>
       </c>
-      <c r="K7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M7" s="5">
+      <c r="K7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" s="10">
         <v>13.43</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="10">
         <v>134.3</v>
       </c>
     </row>
     <row r="8" ht="43.2" spans="1:14">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="7">
         <v>14</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="7">
         <v>14</v>
       </c>
-      <c r="K8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M8" s="5">
+      <c r="K8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" s="10">
         <v>15.45</v>
       </c>
-      <c r="N8" s="5">
+      <c r="N8" s="10">
         <v>216.3</v>
       </c>
     </row>
     <row r="9" ht="43.2" spans="1:14">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="7">
         <v>16</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="7">
         <v>16</v>
       </c>
-      <c r="K9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M9" s="5">
+      <c r="K9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" s="10">
         <v>29.37</v>
       </c>
-      <c r="N9" s="5">
+      <c r="N9" s="10">
         <v>469.92</v>
       </c>
     </row>
     <row r="10" ht="43.2" spans="1:14">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="7">
         <v>6</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="7">
         <v>6</v>
       </c>
-      <c r="K10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M10" s="5">
+      <c r="K10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" s="10">
         <v>30.65</v>
       </c>
-      <c r="N10" s="5">
+      <c r="N10" s="10">
         <v>183.9</v>
       </c>
     </row>
     <row r="11" ht="43.2" spans="1:14">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="7">
         <v>5</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="7">
         <v>5</v>
       </c>
-      <c r="K11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M11" s="5">
+      <c r="K11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" s="10">
         <v>2.74</v>
       </c>
-      <c r="N11" s="5">
+      <c r="N11" s="10">
         <v>13.7</v>
       </c>
     </row>
     <row r="12" ht="43.2" spans="1:14">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="7">
         <v>100</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="7">
         <v>100</v>
       </c>
-      <c r="K12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M12" s="5">
+      <c r="K12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M12" s="10">
         <v>0.17</v>
       </c>
-      <c r="N12" s="5">
+      <c r="N12" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="13" ht="43.2" spans="1:14">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="7">
         <v>100</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="7">
         <v>100</v>
       </c>
-      <c r="K13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M13" s="5">
+      <c r="K13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M13" s="10">
         <v>0.51</v>
       </c>
-      <c r="N13" s="5">
+      <c r="N13" s="10">
         <v>51</v>
       </c>
     </row>
     <row r="14" ht="43.2" spans="1:14">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="7">
         <v>10</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14" s="7">
         <v>10</v>
       </c>
-      <c r="K14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M14" s="5">
+      <c r="K14" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M14" s="10">
         <v>24.5</v>
       </c>
-      <c r="N14" s="5">
+      <c r="N14" s="10">
         <v>245</v>
       </c>
     </row>
     <row r="15" ht="43.2" spans="1:14">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I15" s="7">
         <v>2</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15" s="7">
         <v>2</v>
       </c>
-      <c r="K15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M15" s="5">
+      <c r="K15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M15" s="10">
         <v>0.02</v>
       </c>
-      <c r="N15" s="5">
+      <c r="N15" s="10">
         <v>0.04</v>
       </c>
     </row>
     <row r="16" ht="43.2" spans="1:14">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="7">
         <v>14</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16" s="7">
         <v>14</v>
       </c>
-      <c r="K16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L16" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M16" s="5">
+      <c r="K16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M16" s="10">
         <v>2.03</v>
       </c>
-      <c r="N16" s="5">
+      <c r="N16" s="10">
         <v>28.42</v>
       </c>
     </row>
     <row r="17" ht="43.2" spans="1:14">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="7">
         <v>10</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J17" s="7">
         <v>10</v>
       </c>
-      <c r="K17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M17" s="5">
+      <c r="K17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M17" s="10">
         <v>18.06</v>
       </c>
-      <c r="N17" s="5">
+      <c r="N17" s="10">
         <v>180.6</v>
       </c>
     </row>
     <row r="18" ht="43.2" spans="1:14">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="7">
         <v>17</v>
       </c>
-      <c r="J18" s="2">
+      <c r="J18" s="7">
         <v>17</v>
       </c>
-      <c r="K18" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L18" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M18" s="5">
+      <c r="K18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M18" s="10">
         <v>34.67</v>
       </c>
-      <c r="N18" s="5">
+      <c r="N18" s="10">
         <v>589.39</v>
       </c>
     </row>
     <row r="19" ht="43.2" spans="1:14">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I19" s="7">
         <v>15</v>
       </c>
-      <c r="J19" s="2">
+      <c r="J19" s="7">
         <v>15</v>
       </c>
-      <c r="K19" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M19" s="5">
+      <c r="K19" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L19" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M19" s="10">
         <v>88.88</v>
       </c>
-      <c r="N19" s="5">
+      <c r="N19" s="10">
         <v>1333.2</v>
       </c>
     </row>
     <row r="20" ht="14.4" spans="1:14">
-      <c r="A20" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
+      <c r="A20" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
     </row>
     <row r="21" ht="14.4" spans="1:14">
-      <c r="A21" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="M21" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="N21" s="2" t="s">
+      <c r="A21" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="L21" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="M21" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="N21" s="7" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="22" ht="14.4" spans="1:14">
-      <c r="A22" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="K22" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="L22" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="M22" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="N22" s="5">
+      <c r="A22" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="L22" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="M22" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="N22" s="10">
         <v>4554.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:M6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="5"/>
+  <cols>
+    <col min="1" max="1" width="46.1944444444444" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.0462962962963" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.3333333333333" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.3333333333333" style="1" customWidth="1"/>
+    <col min="5" max="5" width="30.9074074074074" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.47222222222222" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.3333333333333" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6203703703704" style="1" customWidth="1"/>
+    <col min="9" max="9" width="27.6203703703704" style="1" customWidth="1"/>
+    <col min="10" max="10" width="29.1944444444444" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.1944444444444" style="1" customWidth="1"/>
+    <col min="12" max="13" width="31.3333333333333" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="16.8" spans="1:13">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:13">
+      <c r="A2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="4">
+        <v>5</v>
+      </c>
+      <c r="I2" s="4">
+        <v>5</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="3">
+        <v>38.21</v>
+      </c>
+      <c r="M2" s="3">
+        <v>191.05</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" spans="1:13">
+      <c r="A3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="4">
+        <v>34</v>
+      </c>
+      <c r="I3" s="4">
+        <v>34</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="3">
+        <v>3.51</v>
+      </c>
+      <c r="M3" s="3">
+        <v>119.34</v>
+      </c>
+    </row>
+    <row r="4" s="1" customFormat="1" spans="1:1">
+      <c r="A4" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" s="1" customFormat="1" spans="1:13">
+      <c r="A5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" spans="1:13">
+      <c r="A6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="M6" s="3">
+        <v>310.39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="66.1944444444444" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.0462962962963" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.3333333333333" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="16.8" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="3">
+        <v>31.52</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="3">
+        <v>8.85</v>
+      </c>
+    </row>
+    <row r="4" s="1" customFormat="1" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.07</v>
+      </c>
+    </row>
+    <row r="5" s="1" customFormat="1" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="3">
+        <v>10.36</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="1" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="3">
+        <v>7.76</v>
+      </c>
+    </row>
+    <row r="7" s="1" customFormat="1" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="3">
+        <v>8.51</v>
+      </c>
+    </row>
+    <row r="8" s="1" customFormat="1" spans="1:3">
+      <c r="A8" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" s="3">
+        <v>42.24</v>
+      </c>
+    </row>
+    <row r="9" s="1" customFormat="1" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="10" s="1" customFormat="1" spans="1:3">
+      <c r="A10" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="3">
+        <v>107.43</v>
+      </c>
+    </row>
+    <row r="11" s="1" customFormat="1" spans="1:3">
+      <c r="A11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="12" s="1" customFormat="1" spans="1:3">
+      <c r="A12" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="3">
+        <v>62.52</v>
+      </c>
+    </row>
+    <row r="13" s="1" customFormat="1" spans="1:3">
+      <c r="A13" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="3">
+        <v>69.02</v>
+      </c>
+    </row>
+    <row r="14" s="1" customFormat="1" spans="1:3">
+      <c r="A14" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" s="3">
+        <v>6.43</v>
+      </c>
+    </row>
+    <row r="15" s="1" customFormat="1" spans="1:3">
+      <c r="A15" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C15" s="3">
+        <v>5.68</v>
+      </c>
+    </row>
+    <row r="16" s="1" customFormat="1" spans="1:3">
+      <c r="A16" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C16" s="3">
+        <v>2.62</v>
+      </c>
+    </row>
+    <row r="17" s="1" customFormat="1" spans="1:3">
+      <c r="A17" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C17" s="3">
+        <v>3.51</v>
+      </c>
+    </row>
+    <row r="18" s="1" customFormat="1" spans="1:3">
+      <c r="A18" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18" s="3">
+        <v>13.48</v>
+      </c>
+    </row>
+    <row r="19" s="1" customFormat="1" spans="1:3">
+      <c r="A19" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="20" s="1" customFormat="1" spans="1:3">
+      <c r="A20" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20" s="3">
+        <v>11.7</v>
+      </c>
+    </row>
+    <row r="21" s="1" customFormat="1" spans="1:3">
+      <c r="A21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C21" s="3">
+        <v>4.98</v>
+      </c>
+    </row>
+    <row r="22" s="1" customFormat="1" spans="1:3">
+      <c r="A22" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C22" s="3">
+        <v>16.97</v>
+      </c>
+    </row>
+    <row r="23" s="1" customFormat="1" spans="1:3">
+      <c r="A23" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C23" s="3">
+        <v>15.7</v>
+      </c>
+    </row>
+    <row r="24" s="1" customFormat="1" spans="1:1">
+      <c r="A24" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" s="1" customFormat="1" spans="1:3">
+      <c r="A25" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" s="1" customFormat="1" spans="1:3">
+      <c r="A26" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="3">
+        <v>433.04</v>
+      </c>
+    </row>
+    <row r="27" s="1" customFormat="1" spans="1:3">
+      <c r="A27" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>